<commit_message>
Updated file with prices
</commit_message>
<xml_diff>
--- a/Vendors.xlsx
+++ b/Vendors.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24603"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E152BC0C-DEB6-4421-9CCF-FC4083485A79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6488134A-3891-45D9-9095-67DFF677D10D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Vendor 1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="12">
   <si>
     <t>Items</t>
   </si>
@@ -36,6 +36,9 @@
     <t>Quantity</t>
   </si>
   <si>
+    <t>Price</t>
+  </si>
+  <si>
     <t>Milk</t>
   </si>
   <si>
@@ -46,6 +49,9 @@
   </si>
   <si>
     <t xml:space="preserve">Cake </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Price </t>
   </si>
   <si>
     <t>Tooth Paste</t>
@@ -93,8 +99,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -409,7 +416,147 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2">
+        <v>4</v>
+      </c>
+      <c r="E2">
+        <v>3.14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <v>3</v>
+      </c>
+      <c r="E3">
+        <v>2.74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="E5">
+        <v>68</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F502030-2A71-4537-BB08-C98EDF9B91B4}">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3">
+        <v>3</v>
+      </c>
+      <c r="E3">
+        <v>4.99</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>3.61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55774ABA-D8CC-4A1F-A35F-AA77BA70A2D0}">
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F15" sqref="F15"/>
@@ -417,7 +564,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -425,146 +572,48 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="C3">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="E3">
+        <v>2.29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F502030-2A71-4537-BB08-C98EDF9B91B4}">
-  <dimension ref="A1:C5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:C5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55774ABA-D8CC-4A1F-A35F-AA77BA70A2D0}">
-  <dimension ref="A1:C5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C4">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
+      <c r="E4">
+        <v>2.78</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C5">
         <v>50</v>
+      </c>
+      <c r="E5">
+        <v>104.99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added list adding and sheet creating features
</commit_message>
<xml_diff>
--- a/Vendors.xlsx
+++ b/Vendors.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Revature\P0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5ADFF56-8322-4E9F-919D-6526124E46C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{550FD6A2-256F-4258-92AE-D4E6F0CF1942}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1092" yWindow="2016" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Vendor 1" sheetId="1" r:id="rId1"/>
-    <sheet name="Vendor 2" sheetId="2" r:id="rId2"/>
-    <sheet name="Vendor 3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId1"/>
+    <sheet name="Vendor 1" sheetId="1" r:id="rId2"/>
+    <sheet name="Vendor 2" sheetId="2" r:id="rId3"/>
+    <sheet name="Vendor 3" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191028" iterateDelta="1E-4"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="19">
   <si>
     <t>Items</t>
   </si>
@@ -69,6 +70,27 @@
   </si>
   <si>
     <t>Hennessy</t>
+  </si>
+  <si>
+    <t>Vendors</t>
+  </si>
+  <si>
+    <t>Vendor 1</t>
+  </si>
+  <si>
+    <t>Vendor 2</t>
+  </si>
+  <si>
+    <t>Vendor 3</t>
+  </si>
+  <si>
+    <t>Vendor 4</t>
+  </si>
+  <si>
+    <t>Vendor 5</t>
+  </si>
+  <si>
+    <t>Vendor 6</t>
   </si>
 </sst>
 </file>
@@ -420,68 +442,48 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13F2A061-8D1F-4B02-B00A-624341F73EA8}">
+  <dimension ref="A1:A7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2">
-        <v>4</v>
-      </c>
-      <c r="E2">
-        <v>3.14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3">
-        <v>3</v>
-      </c>
-      <c r="E3">
-        <v>2.74</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="E4" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5">
-        <v>2</v>
-      </c>
-      <c r="E5" s="1">
-        <v>68</v>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -490,68 +492,68 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F502030-2A71-4537-BB08-C98EDF9B91B4}">
-  <dimension ref="A1:E5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E5"/>
+      <selection activeCell="C1" sqref="C1:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
       <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>4</v>
+      </c>
+      <c r="C2">
+        <v>3.14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>2.74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="E2" s="1">
-        <v>5.5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3">
-        <v>3</v>
-      </c>
-      <c r="E3">
-        <v>4.99</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <v>3.61</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="E5" s="1">
-        <v>1</v>
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5" s="1">
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -560,67 +562,137 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55774ABA-D8CC-4A1F-A35F-AA77BA70A2D0}">
-  <dimension ref="A1:E5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F502030-2A71-4537-BB08-C98EDF9B91B4}">
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
       <c r="C1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
+      <c r="C2" s="1">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>4.99</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>3.61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5" s="1">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55774ABA-D8CC-4A1F-A35F-AA77BA70A2D0}">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="C2">
+      <c r="B2">
         <v>0</v>
       </c>
-      <c r="E2" s="1">
+      <c r="C2" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
       <c r="C3">
-        <v>3</v>
-      </c>
-      <c r="E3">
         <v>2.29</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>10</v>
       </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
       <c r="C4">
-        <v>2</v>
-      </c>
-      <c r="E4">
         <v>2.78</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>11</v>
       </c>
+      <c r="B5">
+        <v>50</v>
+      </c>
       <c r="C5">
-        <v>50</v>
-      </c>
-      <c r="E5">
         <v>104.99</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updating to Match Excel Branch as a 2ndary backup
</commit_message>
<xml_diff>
--- a/Vendors.xlsx
+++ b/Vendors.xlsx
@@ -1,17 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24326"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Revature\P0\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{550FD6A2-256F-4258-92AE-D4E6F0CF1942}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="1092" yWindow="2016" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Vendor 1" sheetId="1" r:id="rId1"/>
-    <sheet name="Vendor 2" sheetId="2" r:id="rId2"/>
-    <sheet name="Vendor 3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId1"/>
+    <sheet name="Vendor 1" sheetId="1" r:id="rId2"/>
+    <sheet name="Vendor 2" sheetId="2" r:id="rId3"/>
+    <sheet name="Vendor 3" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191028" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -27,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="19">
   <si>
     <t>Items</t>
   </si>
@@ -35,12 +42,21 @@
     <t>Quantity</t>
   </si>
   <si>
+    <t>Price</t>
+  </si>
+  <si>
     <t>Milk</t>
   </si>
   <si>
+    <t>Cookies</t>
+  </si>
+  <si>
     <t>Bananas</t>
   </si>
   <si>
+    <t xml:space="preserve">Cake </t>
+  </si>
+  <si>
     <t xml:space="preserve">Price </t>
   </si>
   <si>
@@ -56,35 +72,33 @@
     <t>Hennessy</t>
   </si>
   <si>
-    <t>Not-Walmart</t>
-  </si>
-  <si>
-    <t>Not-Amazon</t>
-  </si>
-  <si>
-    <t>Not-Target</t>
-  </si>
-  <si>
     <t>Vendors</t>
   </si>
   <si>
-    <t>Not-Starbucks</t>
+    <t>Vendor 1</t>
+  </si>
+  <si>
+    <t>Vendor 2</t>
+  </si>
+  <si>
+    <t>Vendor 3</t>
+  </si>
+  <si>
+    <t>Vendor 4</t>
+  </si>
+  <si>
+    <t>Vendor 5</t>
+  </si>
+  <si>
+    <t>Vendor 6</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -112,10 +126,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -176,7 +189,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -228,7 +241,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -422,119 +435,125 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13F2A061-8D1F-4B02-B00A-624341F73EA8}">
+  <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="2"/>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="2"/>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="2"/>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="C1" sqref="C1:C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
       <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>4</v>
+      </c>
+      <c r="C2">
+        <v>3.14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>2.74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="E2" s="1">
-        <v>5.5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>6</v>
       </c>
-      <c r="C3">
-        <v>3</v>
-      </c>
-      <c r="E3">
-        <v>4.99</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
+      <c r="B5">
         <v>2</v>
       </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <v>3.61</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="E5" s="1">
-        <v>1</v>
+      <c r="C5" s="1">
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -543,64 +562,137 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F502030-2A71-4537-BB08-C98EDF9B91B4}">
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F6"/>
+      <selection activeCell="C1" sqref="C1:C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
       <c r="C1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="C2" s="1">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>4.99</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>3.61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5" s="1">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55774ABA-D8CC-4A1F-A35F-AA77BA70A2D0}">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="E2" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>2.29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4">
         <v>2</v>
       </c>
-      <c r="C3">
-        <v>3</v>
-      </c>
-      <c r="E3">
-        <v>2.29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
       <c r="C4">
-        <v>2</v>
-      </c>
-      <c r="E4">
         <v>2.78</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>11</v>
+      </c>
+      <c r="B5">
+        <v>50</v>
       </c>
       <c r="C5">
-        <v>50</v>
-      </c>
-      <c r="E5">
         <v>104.99</v>
       </c>
     </row>

</xml_diff>